<commit_message>
update propsed method file
</commit_message>
<xml_diff>
--- a/percobaan.xlsx
+++ b/percobaan.xlsx
@@ -480,11 +480,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="371175904"/>
-        <c:axId val="371174816"/>
+        <c:axId val="1242579952"/>
+        <c:axId val="1242570160"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="371175904"/>
+        <c:axId val="1242579952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -541,12 +541,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="371174816"/>
+        <c:crossAx val="1242570160"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="371174816"/>
+        <c:axId val="1242570160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -603,7 +603,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="371175904"/>
+        <c:crossAx val="1242579952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -776,7 +776,7 @@
               <c:size val="5"/>
               <c:spPr>
                 <a:solidFill>
-                  <a:schemeClr val="accent1"/>
+                  <a:srgbClr val="FF0000"/>
                 </a:solidFill>
                 <a:ln w="9525">
                   <a:solidFill>
@@ -827,6 +827,25 @@
             <c:bubble3D val="0"/>
           </c:dPt>
           <c:dPt>
+            <c:idx val="4"/>
+            <c:marker>
+              <c:symbol val="circle"/>
+              <c:size val="5"/>
+              <c:spPr>
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+                <a:ln w="9525">
+                  <a:solidFill>
+                    <a:schemeClr val="accent1"/>
+                  </a:solidFill>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:marker>
+            <c:bubble3D val="0"/>
+          </c:dPt>
+          <c:dPt>
             <c:idx val="7"/>
             <c:marker>
               <c:symbol val="circle"/>
@@ -852,7 +871,7 @@
               <c:size val="5"/>
               <c:spPr>
                 <a:solidFill>
-                  <a:srgbClr val="FF0000"/>
+                  <a:schemeClr val="accent1"/>
                 </a:solidFill>
                 <a:ln w="9525">
                   <a:solidFill>
@@ -890,6 +909,44 @@
               <c:size val="5"/>
               <c:spPr>
                 <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:ln w="9525">
+                  <a:solidFill>
+                    <a:schemeClr val="accent1"/>
+                  </a:solidFill>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:marker>
+            <c:bubble3D val="0"/>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="12"/>
+            <c:marker>
+              <c:symbol val="circle"/>
+              <c:size val="5"/>
+              <c:spPr>
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+                <a:ln w="9525">
+                  <a:solidFill>
+                    <a:schemeClr val="accent1"/>
+                  </a:solidFill>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:marker>
+            <c:bubble3D val="0"/>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="16"/>
+            <c:marker>
+              <c:symbol val="circle"/>
+              <c:size val="5"/>
+              <c:spPr>
+                <a:solidFill>
                   <a:srgbClr val="FF0000"/>
                 </a:solidFill>
                 <a:ln w="9525">
@@ -904,12 +961,12 @@
           </c:dPt>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$M$2:$M$13</c:f>
+              <c:f>Sheet1!$M$2:$M$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="20"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>1</c:v>
@@ -921,40 +978,64 @@
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="6">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>3</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="10">
                   <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$N$2:$N$13</c:f>
+              <c:f>Sheet1!$N$2:$N$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="20"/>
                 <c:pt idx="0">
-                  <c:v>2</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>3</c:v>
@@ -963,31 +1044,55 @@
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>3</c:v>
                 </c:pt>
-                <c:pt idx="4">
-                  <c:v>4</c:v>
-                </c:pt>
                 <c:pt idx="5">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>3</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1002,11 +1107,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="301423072"/>
-        <c:axId val="301436128"/>
+        <c:axId val="1242582672"/>
+        <c:axId val="1242569616"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="301423072"/>
+        <c:axId val="1242582672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1063,12 +1168,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="301436128"/>
+        <c:crossAx val="1242569616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="301436128"/>
+        <c:axId val="1242569616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1125,7 +1230,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="301423072"/>
+        <c:crossAx val="1242582672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2616,8 +2721,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="O17" sqref="O17"/>
+    <sheetView tabSelected="1" topLeftCell="K4" workbookViewId="0">
+      <selection activeCell="W22" sqref="W22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2653,13 +2758,13 @@
         <v>0</v>
       </c>
       <c r="M2">
+        <v>2</v>
+      </c>
+      <c r="N2">
+        <v>3</v>
+      </c>
+      <c r="O2">
         <v>1</v>
-      </c>
-      <c r="N2">
-        <v>2</v>
-      </c>
-      <c r="O2">
-        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
@@ -2716,10 +2821,10 @@
         <v>2</v>
       </c>
       <c r="N5">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="O5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
@@ -2733,13 +2838,13 @@
         <v>0</v>
       </c>
       <c r="M6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N6">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="O6">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
@@ -2756,7 +2861,7 @@
         <v>3</v>
       </c>
       <c r="N7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O7">
         <v>0</v>
@@ -2773,7 +2878,7 @@
         <v>0</v>
       </c>
       <c r="M8">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="N8">
         <v>2</v>
@@ -2793,13 +2898,13 @@
         <v>1</v>
       </c>
       <c r="M9">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="N9">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="O9">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
@@ -2813,13 +2918,13 @@
         <v>0</v>
       </c>
       <c r="M10">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="N10">
         <v>4</v>
       </c>
       <c r="O10">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
@@ -2833,10 +2938,10 @@
         <v>0</v>
       </c>
       <c r="M11">
+        <v>3</v>
+      </c>
+      <c r="N11">
         <v>4</v>
-      </c>
-      <c r="N11">
-        <v>2</v>
       </c>
       <c r="O11">
         <v>1</v>
@@ -2853,13 +2958,13 @@
         <v>0</v>
       </c>
       <c r="M12">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N12">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="O12">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
@@ -2892,6 +2997,15 @@
       <c r="C14">
         <v>1</v>
       </c>
+      <c r="M14">
+        <v>4</v>
+      </c>
+      <c r="N14">
+        <v>2</v>
+      </c>
+      <c r="O14">
+        <v>1</v>
+      </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15">
@@ -2903,6 +3017,15 @@
       <c r="C15">
         <v>1</v>
       </c>
+      <c r="M15">
+        <v>5</v>
+      </c>
+      <c r="N15">
+        <v>2</v>
+      </c>
+      <c r="O15">
+        <v>0</v>
+      </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16">
@@ -2914,8 +3037,17 @@
       <c r="C16">
         <v>0</v>
       </c>
+      <c r="M16">
+        <v>3</v>
+      </c>
+      <c r="N16">
+        <v>2</v>
+      </c>
+      <c r="O16">
+        <v>0</v>
+      </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>4</v>
       </c>
@@ -2925,8 +3057,17 @@
       <c r="C17">
         <v>0</v>
       </c>
+      <c r="M17">
+        <v>4</v>
+      </c>
+      <c r="N17">
+        <v>1</v>
+      </c>
+      <c r="O17">
+        <v>0</v>
+      </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>4</v>
       </c>
@@ -2936,8 +3077,17 @@
       <c r="C18">
         <v>1</v>
       </c>
+      <c r="M18">
+        <v>4</v>
+      </c>
+      <c r="N18">
+        <v>3</v>
+      </c>
+      <c r="O18">
+        <v>1</v>
+      </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>4</v>
       </c>
@@ -2947,8 +3097,17 @@
       <c r="C19">
         <v>1</v>
       </c>
+      <c r="M19">
+        <v>5</v>
+      </c>
+      <c r="N19">
+        <v>3</v>
+      </c>
+      <c r="O19">
+        <v>0</v>
+      </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>4</v>
       </c>
@@ -2958,8 +3117,17 @@
       <c r="C20">
         <v>0</v>
       </c>
+      <c r="M20">
+        <v>4</v>
+      </c>
+      <c r="N20">
+        <v>4</v>
+      </c>
+      <c r="O20">
+        <v>0</v>
+      </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>4</v>
       </c>
@@ -2969,8 +3137,17 @@
       <c r="C21">
         <v>0</v>
       </c>
+      <c r="M21">
+        <v>5</v>
+      </c>
+      <c r="N21">
+        <v>2</v>
+      </c>
+      <c r="O21">
+        <v>0</v>
+      </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>5</v>
       </c>
@@ -2981,7 +3158,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>5</v>
       </c>
@@ -2992,7 +3169,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>5</v>
       </c>
@@ -3003,7 +3180,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>5</v>
       </c>
@@ -3014,7 +3191,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>5</v>
       </c>

</xml_diff>